<commit_message>
Performs tare after calibration.
</commit_message>
<xml_diff>
--- a/doc/orcamento.xlsx
+++ b/doc/orcamento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glber\ownCloud\workspace-git\wxPython\P003-GUI-BancadaTestesEstaticos\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E022A2D7-D68B-427B-9F40-8BFA908AE2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53BD3A1-8A1A-4DB3-B5BF-5217D17AEC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4A525F49-ED3C-446B-AB30-19B718C9377D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Componentes</t>
   </si>
@@ -48,16 +48,7 @@
     <t>Amplificador HX711</t>
   </si>
   <si>
-    <t>Placa ilhada</t>
-  </si>
-  <si>
-    <t>Conector USB</t>
-  </si>
-  <si>
     <t>Cabo USB-mini USB</t>
-  </si>
-  <si>
-    <t>Cabo USB-USB-tipoB</t>
   </si>
   <si>
     <t>Impressão 3D</t>
@@ -73,6 +64,18 @@
   </si>
   <si>
     <t>Aliexpress</t>
+  </si>
+  <si>
+    <t>Célula de carga</t>
+  </si>
+  <si>
+    <t>Cabo USB-USB-tipoB (por célula de carga)</t>
+  </si>
+  <si>
+    <t>Placa ilhada (7cm x 9cm)</t>
+  </si>
+  <si>
+    <t>Conector USB tipo B</t>
   </si>
 </sst>
 </file>
@@ -159,9 +162,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -199,7 +202,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -305,7 +308,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -447,7 +450,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1685,15 +1688,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75144390-9702-42B6-973D-F049C9A54390}">
-  <dimension ref="A2:C11"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C11"/>
+      <selection activeCell="A3" sqref="A3:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="1" max="1" width="35.77734375" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="12.77734375" customWidth="1"/>
   </cols>
@@ -1703,10 +1706,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1733,80 +1736,87 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
         <v>2</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C7" s="3">
-        <v>4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="3">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B10" s="3">
-        <v>0.2</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3">
-        <v>0.2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4">
-        <f>SUM(B3:B10)</f>
+        <v>5</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4">
+        <f>SUM(B3:B11)</f>
         <v>102.2</v>
       </c>
-      <c r="C11" s="3">
-        <f>SUM(C3:C10)</f>
+      <c r="C12" s="3">
+        <f>SUM(C3:C11)</f>
         <v>50.800000000000004</v>
       </c>
     </row>

</xml_diff>